<commit_message>
Modificaciones en los repoertes
</commit_message>
<xml_diff>
--- a/protected/modules/excel/templates/EvaluacionPorCompetenciasTemplate_AC.xlsx
+++ b/protected/modules/excel/templates/EvaluacionPorCompetenciasTemplate_AC.xlsx
@@ -258,17 +258,11 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -292,6 +286,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1014,11 +1014,11 @@
         </c:dLbls>
         <c:gapWidth val="355"/>
         <c:overlap val="-70"/>
-        <c:axId val="120137176"/>
-        <c:axId val="166993296"/>
+        <c:axId val="166571584"/>
+        <c:axId val="166151496"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="120137176"/>
+        <c:axId val="166571584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1061,7 +1061,7 @@
             <a:endParaRPr lang="es-CR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="166993296"/>
+        <c:crossAx val="166151496"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1069,7 +1069,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="166993296"/>
+        <c:axId val="166151496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1187,7 +1187,7 @@
             <a:endParaRPr lang="es-CR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="120137176"/>
+        <c:crossAx val="166571584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1289,11 +1289,11 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="70" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -1302,7 +1302,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="es-MX" cap="all" baseline="0"/>
+              <a:rPr lang="es-MX"/>
               <a:t>Análisis de cobertura de Requisitos</a:t>
             </a:r>
           </a:p>
@@ -1322,11 +1322,11 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="70" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
@@ -1359,42 +1359,17 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:gradFill rotWithShape="1">
-              <a:gsLst>
-                <a:gs pos="0">
-                  <a:schemeClr val="accent3">
-                    <a:satMod val="103000"/>
-                    <a:lumMod val="102000"/>
-                    <a:tint val="94000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="50000">
-                  <a:schemeClr val="accent3">
-                    <a:satMod val="110000"/>
-                    <a:lumMod val="100000"/>
-                    <a:shade val="100000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="100000">
-                  <a:schemeClr val="accent3">
-                    <a:lumMod val="99000"/>
-                    <a:satMod val="120000"/>
-                    <a:shade val="78000"/>
-                  </a:schemeClr>
-                </a:gs>
-              </a:gsLst>
-              <a:lin ang="5400000" scaled="0"/>
-            </a:gradFill>
-            <a:ln>
-              <a:noFill/>
+            <a:solidFill>
+              <a:schemeClr val="accent3">
+                <a:alpha val="10196"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln w="50800">
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
             </a:ln>
-            <a:effectLst>
-              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-                <a:srgbClr val="000000">
-                  <a:alpha val="63000"/>
-                </a:srgbClr>
-              </a:outerShdw>
-            </a:effectLst>
+            <a:effectLst/>
           </c:spPr>
           <c:cat>
             <c:strRef>
@@ -1447,42 +1422,19 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:gradFill rotWithShape="1">
-              <a:gsLst>
-                <a:gs pos="0">
-                  <a:schemeClr val="accent4">
-                    <a:satMod val="103000"/>
-                    <a:lumMod val="102000"/>
-                    <a:tint val="94000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="50000">
-                  <a:schemeClr val="accent4">
-                    <a:satMod val="110000"/>
-                    <a:lumMod val="100000"/>
-                    <a:shade val="100000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="100000">
-                  <a:schemeClr val="accent4">
-                    <a:lumMod val="99000"/>
-                    <a:satMod val="120000"/>
-                    <a:shade val="78000"/>
-                  </a:schemeClr>
-                </a:gs>
-              </a:gsLst>
-              <a:lin ang="5400000" scaled="0"/>
-            </a:gradFill>
-            <a:ln>
-              <a:noFill/>
+            <a:solidFill>
+              <a:schemeClr val="accent4">
+                <a:alpha val="10196"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln w="50800">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
             </a:ln>
-            <a:effectLst>
-              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-                <a:srgbClr val="000000">
-                  <a:alpha val="63000"/>
-                </a:srgbClr>
-              </a:outerShdw>
-            </a:effectLst>
+            <a:effectLst/>
           </c:spPr>
           <c:cat>
             <c:strRef>
@@ -1519,11 +1471,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="167026096"/>
-        <c:axId val="167441128"/>
+        <c:axId val="190032504"/>
+        <c:axId val="190032888"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="167026096"/>
+        <c:axId val="190032504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1535,9 +1487,9 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
+              <a:schemeClr val="dk1">
                 <a:lumMod val="15000"/>
                 <a:lumOff val="85000"/>
               </a:schemeClr>
@@ -1553,9 +1505,9 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -1566,7 +1518,7 @@
             <a:endParaRPr lang="es-CR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="167441128"/>
+        <c:crossAx val="190032888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1574,7 +1526,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="167441128"/>
+        <c:axId val="190032888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1584,7 +1536,7 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="tx1">
+                <a:schemeClr val="dk1">
                   <a:lumMod val="15000"/>
                   <a:lumOff val="85000"/>
                 </a:schemeClr>
@@ -1612,9 +1564,9 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -1625,7 +1577,7 @@
             <a:endParaRPr lang="es-CR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="167026096"/>
+        <c:crossAx val="190032504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1655,9 +1607,9 @@
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
@@ -1674,12 +1626,25 @@
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="100000">
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="43000">
+          <a:schemeClr val="lt1"/>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
-        <a:schemeClr val="tx1">
+        <a:schemeClr val="dk1">
           <a:lumMod val="15000"/>
           <a:lumOff val="85000"/>
         </a:schemeClr>
@@ -1740,9 +1705,10 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="es-CR"/>
-              <a:t>Comparación entre AC y ECE</a:t>
+              <a:rPr lang="es-CR" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0"/>
+              <a:t>Aporte de AC (60%) y ECE (40%) a la calificación</a:t>
             </a:r>
+            <a:endParaRPr lang="es-CR"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -1835,11 +1801,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="167404240"/>
-        <c:axId val="167465696"/>
+        <c:axId val="165158720"/>
+        <c:axId val="165159112"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="167404240"/>
+        <c:axId val="165158720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1882,7 +1848,7 @@
             <a:endParaRPr lang="es-CR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="167465696"/>
+        <c:crossAx val="165159112"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1890,7 +1856,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="167465696"/>
+        <c:axId val="165159112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1941,7 +1907,7 @@
             <a:endParaRPr lang="es-CR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="167404240"/>
+        <c:crossAx val="165158720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2708,33 +2674,33 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="351">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="319">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
@@ -2744,20 +2710,33 @@
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="100000">
+            <a:schemeClr val="lt1">
+              <a:lumMod val="95000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="43000">
+            <a:schemeClr val="lt1"/>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
@@ -2772,9 +2751,9 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -2791,16 +2770,11 @@
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="lt1"/>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
       </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
     <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
@@ -2808,72 +2782,107 @@
     </cs:bodyPr>
   </cs:dataLabelCallout>
   <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="3">
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
-    </cs:fontRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="10196"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="50800">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="30000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="3">
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
-    </cs:fontRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="10196"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="50800">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="30000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="3"/>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="34925" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="50800" cap="rnd" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="30000"/>
+          </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dataPointLine>
   <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="3">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="4"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="3"/>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -2889,16 +2898,15 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
@@ -2913,20 +2921,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -2940,14 +2948,13 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dropLine>
@@ -2959,14 +2966,13 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:errorBar>
@@ -2975,7 +2981,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:floor>
   <cs:gridlineMajor>
@@ -2988,7 +2994,7 @@
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
@@ -3007,7 +3013,7 @@
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="5000"/>
             <a:lumOff val="95000"/>
           </a:schemeClr>
@@ -3024,33 +3030,31 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
       </a:ln>
     </cs:spPr>
   </cs:leaderLine>
@@ -3059,9 +3063,9 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -3071,7 +3075,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:plotArea>
   <cs:plotArea3D>
@@ -3079,7 +3083,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:plotArea3D>
   <cs:seriesAxis>
@@ -3088,19 +3092,18 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -3113,14 +3116,13 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:seriesLine>
@@ -3129,27 +3131,30 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1600" b="1" kern="1200" baseline="0"/>
+    <cs:defRPr sz="1600" b="0" kern="1200" spc="70" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
+      <cs:styleClr val="0"/>
     </cs:lnRef>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="63500" cap="rnd" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -3158,9 +3163,9 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -3170,7 +3175,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -3178,9 +3183,9 @@
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -3191,9 +3196,9 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -3203,7 +3208,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:wall>
 </cs:chartStyle>
@@ -4072,8 +4077,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6:K6"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="L33" sqref="L33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4092,109 +4097,109 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="27"/>
       <c r="M1" s="11"/>
     </row>
     <row r="2" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
-      <c r="K2" s="18"/>
-      <c r="L2" s="18"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
+      <c r="K2" s="28"/>
+      <c r="L2" s="28"/>
       <c r="M2" s="12"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="19"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
       <c r="G4" s="9"/>
-      <c r="H4" s="19" t="s">
+      <c r="H4" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="19"/>
-      <c r="J4" s="28"/>
-      <c r="K4" s="28"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="26"/>
+      <c r="K4" s="26"/>
       <c r="L4" s="1"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C5" s="19" t="s">
+      <c r="C5" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="19"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
       <c r="G5" s="9"/>
-      <c r="H5" s="19" t="s">
+      <c r="H5" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="I5" s="19"/>
-      <c r="J5" s="28"/>
-      <c r="K5" s="28"/>
+      <c r="I5" s="18"/>
+      <c r="J5" s="26"/>
+      <c r="K5" s="26"/>
       <c r="L5" s="1"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
       <c r="G6" s="9"/>
-      <c r="H6" s="19" t="s">
+      <c r="H6" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="I6" s="19"/>
-      <c r="J6" s="28"/>
-      <c r="K6" s="28"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="26"/>
+      <c r="K6" s="26"/>
       <c r="L6" s="1"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
       <c r="G7" s="9"/>
-      <c r="K7" s="21"/>
-      <c r="L7" s="21"/>
+      <c r="K7" s="19"/>
+      <c r="L7" s="19"/>
     </row>
     <row r="8" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="18"/>
-      <c r="J8" s="18"/>
-      <c r="K8" s="18"/>
-      <c r="L8" s="18"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="28"/>
+      <c r="I8" s="28"/>
+      <c r="J8" s="28"/>
+      <c r="K8" s="28"/>
+      <c r="L8" s="28"/>
       <c r="M8" s="12"/>
     </row>
     <row r="47" spans="6:7" x14ac:dyDescent="0.25">
@@ -4214,10 +4219,10 @@
       </c>
     </row>
     <row r="49" spans="5:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="E49" s="23" t="s">
+      <c r="E49" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="F49" s="24"/>
+      <c r="F49" s="22"/>
       <c r="G49" s="13" t="s">
         <v>16</v>
       </c>
@@ -4232,10 +4237,10 @@
       </c>
     </row>
     <row r="50" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E50" s="25" t="s">
+      <c r="E50" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="F50" s="26"/>
+      <c r="F50" s="24"/>
       <c r="G50" s="14"/>
       <c r="H50" s="3">
         <v>2</v>
@@ -4246,10 +4251,10 @@
       <c r="J50" s="4"/>
     </row>
     <row r="51" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E51" s="22" t="s">
+      <c r="E51" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="F51" s="22"/>
+      <c r="F51" s="20"/>
       <c r="G51" s="15"/>
       <c r="H51" s="3">
         <v>2</v>
@@ -4260,10 +4265,10 @@
       <c r="J51" s="4"/>
     </row>
     <row r="52" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E52" s="22" t="s">
+      <c r="E52" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="F52" s="22"/>
+      <c r="F52" s="20"/>
       <c r="G52" s="15"/>
       <c r="H52" s="3">
         <v>3</v>
@@ -4274,56 +4279,56 @@
       <c r="J52" s="4"/>
     </row>
     <row r="53" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E53" s="22"/>
-      <c r="F53" s="22"/>
+      <c r="E53" s="20"/>
+      <c r="F53" s="20"/>
       <c r="G53" s="15"/>
       <c r="H53" s="3"/>
       <c r="I53" s="4"/>
       <c r="J53" s="4"/>
     </row>
     <row r="54" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E54" s="22"/>
-      <c r="F54" s="22"/>
+      <c r="E54" s="20"/>
+      <c r="F54" s="20"/>
       <c r="G54" s="15"/>
       <c r="H54" s="3"/>
       <c r="I54" s="4"/>
       <c r="J54" s="4"/>
     </row>
     <row r="55" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E55" s="22"/>
-      <c r="F55" s="22"/>
+      <c r="E55" s="20"/>
+      <c r="F55" s="20"/>
       <c r="G55" s="15"/>
       <c r="H55" s="3"/>
       <c r="I55" s="4"/>
       <c r="J55" s="4"/>
     </row>
     <row r="56" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E56" s="22"/>
-      <c r="F56" s="22"/>
+      <c r="E56" s="20"/>
+      <c r="F56" s="20"/>
       <c r="G56" s="15"/>
       <c r="H56" s="3"/>
       <c r="I56" s="4"/>
       <c r="J56" s="4"/>
     </row>
     <row r="57" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E57" s="22"/>
-      <c r="F57" s="22"/>
+      <c r="E57" s="20"/>
+      <c r="F57" s="20"/>
       <c r="G57" s="15"/>
       <c r="H57" s="3"/>
       <c r="I57" s="4"/>
       <c r="J57" s="4"/>
     </row>
     <row r="58" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E58" s="22"/>
-      <c r="F58" s="22"/>
+      <c r="E58" s="20"/>
+      <c r="F58" s="20"/>
       <c r="G58" s="15"/>
       <c r="H58" s="5"/>
       <c r="I58" s="4"/>
       <c r="J58" s="4"/>
     </row>
     <row r="59" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E59" s="22"/>
-      <c r="F59" s="22"/>
+      <c r="E59" s="20"/>
+      <c r="F59" s="20"/>
       <c r="G59" s="15"/>
       <c r="H59" s="7"/>
       <c r="I59" s="4"/>
@@ -4338,16 +4343,30 @@
       <c r="J60" s="6"/>
     </row>
     <row r="62" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E62" s="20" t="s">
+      <c r="E62" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="F62" s="20"/>
-      <c r="G62" s="27"/>
-      <c r="H62" s="27"/>
+      <c r="F62" s="17"/>
+      <c r="G62" s="25"/>
+      <c r="H62" s="25"/>
       <c r="I62" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A2:L2"/>
+    <mergeCell ref="A8:L8"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
     <mergeCell ref="E62:F62"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="K7:L7"/>
@@ -4364,20 +4383,6 @@
     <mergeCell ref="E57:F57"/>
     <mergeCell ref="E58:F58"/>
     <mergeCell ref="E7:F7"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A2:L2"/>
-    <mergeCell ref="A8:L8"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="55" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
Modificación de templates de reportes con AC
</commit_message>
<xml_diff>
--- a/protected/modules/excel/templates/EvaluacionPorCompetenciasTemplate_AC.xlsx
+++ b/protected/modules/excel/templates/EvaluacionPorCompetenciasTemplate_AC.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Hoja1!$A$1:$I$87</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Hoja1!$A$1:$I$69</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Modelo de Gestión por Competencias</t>
   </si>
@@ -77,12 +77,6 @@
     <t>Promedio ponderado</t>
   </si>
   <si>
-    <t>AC</t>
-  </si>
-  <si>
-    <t>ECE</t>
-  </si>
-  <si>
     <t>Método seleccionado</t>
   </si>
   <si>
@@ -100,12 +94,18 @@
   <si>
     <t>Detalle AC</t>
   </si>
+  <si>
+    <t>Evaluación AC</t>
+  </si>
+  <si>
+    <t>Evaluación mediante Entrevista Conductual Estructurada y Assessment Center  con proporciones 40% y 60% respectivamente.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -191,8 +191,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -205,14 +212,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -327,11 +328,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -391,12 +403,31 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -420,66 +451,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="12" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="12" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="12" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="12">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="8"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -696,6 +684,40 @@
         </bottom>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="8"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -754,6 +776,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -775,7 +798,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$G$56</c:f>
+              <c:f>Hoja1!$G$38</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -796,7 +819,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Hoja1!$B$57:$B$65</c:f>
+              <c:f>Hoja1!$B$39:$B$47</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -813,7 +836,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$G$57:$G$65</c:f>
+              <c:f>Hoja1!$G$39:$G$47</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -850,7 +873,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$H$56</c:f>
+              <c:f>Hoja1!$H$38</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -871,7 +894,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Hoja1!$B$57:$B$65</c:f>
+              <c:f>Hoja1!$B$39:$B$47</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -888,7 +911,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$H$57:$H$65</c:f>
+              <c:f>Hoja1!$H$39:$H$47</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -930,11 +953,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="164926888"/>
-        <c:axId val="164927272"/>
+        <c:axId val="229017320"/>
+        <c:axId val="230032632"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="164926888"/>
+        <c:axId val="229017320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -977,7 +1000,7 @@
             <a:endParaRPr lang="es-CR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="164927272"/>
+        <c:crossAx val="230032632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -985,7 +1008,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="164927272"/>
+        <c:axId val="230032632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1031,6 +1054,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1071,7 +1095,7 @@
             <a:endParaRPr lang="es-CR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="164926888"/>
+        <c:crossAx val="229017320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1085,6 +1109,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1164,6 +1189,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1204,7 +1230,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$G$56</c:f>
+              <c:f>Hoja1!$G$38</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1227,7 +1253,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Hoja1!$B$57:$B$65</c:f>
+              <c:f>Hoja1!$B$39:$B$47</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1244,7 +1270,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$G$57:$G$65</c:f>
+              <c:f>Hoja1!$G$39:$G$47</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -1281,7 +1307,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$H$56</c:f>
+              <c:f>Hoja1!$H$38</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1304,7 +1330,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Hoja1!$B$57:$B$65</c:f>
+              <c:f>Hoja1!$B$39:$B$47</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1321,7 +1347,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$H$57:$H$65</c:f>
+              <c:f>Hoja1!$H$39:$H$47</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -1361,11 +1387,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="190417488"/>
-        <c:axId val="190417872"/>
+        <c:axId val="230033416"/>
+        <c:axId val="230033808"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="190417488"/>
+        <c:axId val="230033416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1408,7 +1434,7 @@
             <a:endParaRPr lang="es-CR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="190417872"/>
+        <c:crossAx val="230033808"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1416,7 +1442,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="190417872"/>
+        <c:axId val="230033808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1467,7 +1493,7 @@
             <a:endParaRPr lang="es-CR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="190417488"/>
+        <c:crossAx val="230033416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1481,6 +1507,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1547,337 +1574,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="es-CR" sz="1400" b="0" i="0" baseline="0">
-                <a:effectLst/>
-              </a:rPr>
-              <a:t>Aporte de AC (60%) y ECE (40%) a la calificación</a:t>
-            </a:r>
-            <a:endParaRPr lang="es-CR" sz="1400">
-              <a:effectLst/>
-            </a:endParaRPr>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="es-CR"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Hoja1!$D$50:$E$50</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>AC</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>ECE</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Hoja1!$D$51:$E$51</c:f>
-              <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="190390816"/>
-        <c:axId val="190391200"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="190390816"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="es-CR"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="190391200"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="190391200"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="es-CR"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="190390816"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="es-CR"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup orientation="portrait"/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -2422,522 +2119,19 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>185738</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1438275</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>85726</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2961,13 +2155,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>57149</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>4760</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>1038225</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2987,50 +2181,20 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>514347</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>9524</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>723899</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B56:H65" totalsRowShown="0" headerRowDxfId="0" dataDxfId="10" headerRowBorderDxfId="11" tableBorderDxfId="9" totalsRowBorderDxfId="8">
-  <autoFilter ref="B56:H65"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B38:H47" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8" totalsRowBorderDxfId="7">
+  <autoFilter ref="B38:H47"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Méritos y Habilidades" dataDxfId="7"/>
-    <tableColumn id="2" name="Variable equivalente (VE)" dataDxfId="6"/>
-    <tableColumn id="3" name="Método seleccionado" dataDxfId="5"/>
-    <tableColumn id="8" name="Calificación VE" dataDxfId="4"/>
-    <tableColumn id="4" name="Valor Relativo" dataDxfId="3"/>
-    <tableColumn id="5" name="Candidato Ideal" dataDxfId="2"/>
-    <tableColumn id="6" name="Calificación" dataDxfId="1"/>
+    <tableColumn id="1" name="Méritos y Habilidades" dataDxfId="6"/>
+    <tableColumn id="2" name="Variable equivalente (VE)" dataDxfId="5"/>
+    <tableColumn id="3" name="Método seleccionado" dataDxfId="4"/>
+    <tableColumn id="8" name="Calificación VE" dataDxfId="3"/>
+    <tableColumn id="4" name="Valor Relativo" dataDxfId="2"/>
+    <tableColumn id="5" name="Candidato Ideal" dataDxfId="1"/>
+    <tableColumn id="6" name="Calificación" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3299,10 +2463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M81"/>
+  <dimension ref="A1:M63"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="B56" sqref="B56:H56"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3323,437 +2487,405 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
       <c r="J1" s="4"/>
       <c r="K1" s="4"/>
       <c r="L1" s="4"/>
       <c r="M1" s="4"/>
     </row>
     <row r="2" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35"/>
+      <c r="B2" s="40"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
       <c r="J2" s="5"/>
       <c r="K2" s="5"/>
       <c r="L2" s="5"/>
       <c r="M2" s="5"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="36"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="36" t="s">
+      <c r="B4" s="41"/>
+      <c r="C4" s="42"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="36"/>
-      <c r="G4" s="37"/>
-      <c r="H4" s="37"/>
+      <c r="F4" s="41"/>
+      <c r="G4" s="42"/>
+      <c r="H4" s="42"/>
       <c r="I4" s="18"/>
       <c r="J4" s="19"/>
       <c r="K4" s="18"/>
       <c r="L4" s="1"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="36" t="s">
+      <c r="A5" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="36"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="36" t="s">
+      <c r="B5" s="41"/>
+      <c r="C5" s="42"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="36"/>
-      <c r="G5" s="37"/>
-      <c r="H5" s="37"/>
+      <c r="F5" s="41"/>
+      <c r="G5" s="42"/>
+      <c r="H5" s="42"/>
       <c r="I5" s="18"/>
       <c r="J5" s="19"/>
       <c r="K5" s="19"/>
       <c r="L5" s="1"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B6" s="42"/>
-      <c r="C6" s="42"/>
+      <c r="B6" s="32"/>
+      <c r="C6" s="32"/>
       <c r="D6" s="1"/>
-      <c r="E6" s="36" t="s">
+      <c r="E6" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="36"/>
-      <c r="G6" s="37"/>
-      <c r="H6" s="37"/>
+      <c r="F6" s="41"/>
+      <c r="G6" s="42"/>
+      <c r="H6" s="42"/>
       <c r="I6" s="18"/>
       <c r="J6" s="19"/>
       <c r="K6" s="18"/>
       <c r="L6" s="1"/>
     </row>
-    <row r="8" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="35" t="s">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B7" s="29"/>
+      <c r="C7" s="29"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="28"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="18"/>
+      <c r="L7" s="1"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B8" s="46" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="46"/>
+      <c r="D8" s="46"/>
+      <c r="E8" s="46"/>
+      <c r="F8" s="46"/>
+      <c r="G8" s="46"/>
+      <c r="H8" s="46"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="18"/>
+      <c r="L8" s="1"/>
+    </row>
+    <row r="10" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="35"/>
-      <c r="C8" s="35"/>
-      <c r="D8" s="35"/>
-      <c r="E8" s="35"/>
-      <c r="F8" s="35"/>
-      <c r="G8" s="35"/>
-      <c r="H8" s="35"/>
-      <c r="I8" s="35"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
-    </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B35" s="29"/>
-    </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B36" s="41"/>
-    </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B37" s="41"/>
-      <c r="C37" s="28"/>
-    </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B38" s="41"/>
-      <c r="C38" s="28"/>
-    </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B39" s="41"/>
-      <c r="C39" s="28"/>
-    </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B40" s="28"/>
-    </row>
-    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D49" s="15"/>
-      <c r="E49" s="15"/>
-      <c r="F49" s="13"/>
-      <c r="G49" s="13" t="s">
+      <c r="B10" s="40"/>
+      <c r="C10" s="40"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="40"/>
+      <c r="H10" s="40"/>
+      <c r="I10" s="40"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="F33" s="13"/>
+      <c r="G33" s="13"/>
+      <c r="H33" s="13"/>
+      <c r="I33" s="13"/>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C34" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="D34" s="43"/>
+      <c r="E34" s="44"/>
+      <c r="F34" s="44"/>
+      <c r="G34" s="45"/>
+      <c r="H34" s="13"/>
+      <c r="I34" s="13"/>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C35" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="D35" s="38"/>
+      <c r="E35" s="38"/>
+      <c r="F35" s="38"/>
+      <c r="G35" s="38"/>
+      <c r="H35" s="13"/>
+      <c r="I35" s="13"/>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C36" s="37"/>
+      <c r="D36" s="38"/>
+      <c r="E36" s="38"/>
+      <c r="F36" s="38"/>
+      <c r="G36" s="38"/>
+      <c r="H36" s="13"/>
+      <c r="I36" s="13"/>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D37" s="15"/>
+      <c r="E37" s="15"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="13"/>
+      <c r="H37" s="13"/>
+      <c r="I37" s="13"/>
+    </row>
+    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B38" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="C38" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="D38" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="H49" s="13" t="s">
+      <c r="E38" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="I49" s="13"/>
-    </row>
-    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D50" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="E50" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="F50" s="13"/>
-      <c r="G50" s="13">
+      <c r="F38" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="G38" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="H38" s="30" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B39" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C39" s="16"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="6"/>
+      <c r="F39" s="23">
         <v>2</v>
       </c>
-      <c r="H50" s="13">
+      <c r="G39" s="23">
+        <v>2</v>
+      </c>
+      <c r="H39" s="24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B40" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C40" s="16"/>
+      <c r="D40" s="6"/>
+      <c r="E40" s="6"/>
+      <c r="F40" s="23">
+        <v>2</v>
+      </c>
+      <c r="G40" s="23">
+        <v>2</v>
+      </c>
+      <c r="H40" s="24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B41" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C41" s="16"/>
+      <c r="D41" s="7"/>
+      <c r="E41" s="7"/>
+      <c r="F41" s="25">
+        <v>3</v>
+      </c>
+      <c r="G41" s="25">
+        <v>3</v>
+      </c>
+      <c r="H41" s="26">
         <v>1</v>
       </c>
-      <c r="I50" s="13"/>
-    </row>
-    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D51" s="27">
+    </row>
+    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B42" s="16"/>
+      <c r="C42" s="16"/>
+      <c r="D42" s="7"/>
+      <c r="E42" s="7"/>
+      <c r="F42" s="23"/>
+      <c r="G42" s="23">
+        <v>4</v>
+      </c>
+      <c r="H42" s="24">
         <v>2</v>
       </c>
-      <c r="E51" s="27">
-        <v>1</v>
-      </c>
-      <c r="F51" s="13"/>
-      <c r="G51" s="13"/>
-      <c r="H51" s="13"/>
-      <c r="I51" s="13"/>
-    </row>
-    <row r="52" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D52" s="30"/>
-      <c r="E52" s="30"/>
-      <c r="F52" s="13"/>
-      <c r="G52" s="13"/>
-      <c r="H52" s="13"/>
-      <c r="I52" s="13"/>
-    </row>
-    <row r="53" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C53" s="31" t="s">
-        <v>23</v>
-      </c>
-      <c r="D53" s="33"/>
-      <c r="E53" s="33"/>
-      <c r="F53" s="33"/>
-      <c r="G53" s="33"/>
-      <c r="H53" s="13"/>
-      <c r="I53" s="13"/>
-    </row>
-    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C54" s="32"/>
-      <c r="D54" s="33"/>
-      <c r="E54" s="33"/>
-      <c r="F54" s="33"/>
-      <c r="G54" s="33"/>
-      <c r="H54" s="13"/>
-      <c r="I54" s="13"/>
-    </row>
-    <row r="55" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D55" s="15"/>
-      <c r="E55" s="15"/>
-      <c r="F55" s="13"/>
-      <c r="G55" s="13"/>
-      <c r="H55" s="13"/>
-      <c r="I55" s="13"/>
-    </row>
-    <row r="56" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B56" s="43" t="s">
-        <v>8</v>
-      </c>
-      <c r="C56" s="43" t="s">
+    </row>
+    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B43" s="16"/>
+      <c r="C43" s="16"/>
+      <c r="D43" s="7"/>
+      <c r="E43" s="7"/>
+      <c r="F43" s="23"/>
+      <c r="G43" s="23">
+        <v>3</v>
+      </c>
+      <c r="H43" s="24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B44" s="16"/>
+      <c r="C44" s="16"/>
+      <c r="D44" s="7"/>
+      <c r="E44" s="7"/>
+      <c r="F44" s="23"/>
+      <c r="G44" s="23">
+        <v>2</v>
+      </c>
+      <c r="H44" s="24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B45" s="10"/>
+      <c r="C45" s="16"/>
+      <c r="D45" s="7"/>
+      <c r="E45" s="7"/>
+      <c r="F45" s="23"/>
+      <c r="G45" s="23">
+        <v>2</v>
+      </c>
+      <c r="H45" s="24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B46" s="10"/>
+      <c r="C46" s="16"/>
+      <c r="D46" s="7"/>
+      <c r="E46" s="7"/>
+      <c r="F46" s="25"/>
+      <c r="G46" s="25">
+        <v>3</v>
+      </c>
+      <c r="H46" s="26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B47" s="10"/>
+      <c r="C47" s="10"/>
+      <c r="D47" s="10"/>
+      <c r="E47" s="10"/>
+      <c r="F47" s="25"/>
+      <c r="G47" s="25"/>
+      <c r="H47" s="26"/>
+    </row>
+    <row r="48" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B48" s="9"/>
+      <c r="C48" s="20"/>
+      <c r="D48" s="9"/>
+      <c r="E48" s="9"/>
+      <c r="F48" s="14"/>
+      <c r="G48" s="14"/>
+      <c r="H48" s="14"/>
+    </row>
+    <row r="49" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B49" s="9"/>
+      <c r="C49" s="20"/>
+      <c r="D49" s="9"/>
+      <c r="E49" s="9"/>
+      <c r="F49" s="14"/>
+      <c r="G49" s="14"/>
+      <c r="H49" s="14"/>
+    </row>
+    <row r="50" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B50" s="9"/>
+      <c r="C50" s="20"/>
+      <c r="D50" s="9"/>
+      <c r="E50" s="9"/>
+      <c r="F50" s="14"/>
+      <c r="G50" s="14"/>
+      <c r="H50" s="14"/>
+    </row>
+    <row r="51" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="8"/>
+      <c r="G51" s="9"/>
+      <c r="H51" s="14"/>
+      <c r="I51" s="14"/>
+      <c r="J51" s="14"/>
+    </row>
+    <row r="52" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D52" s="8"/>
+      <c r="E52" s="8"/>
+      <c r="F52" s="8"/>
+      <c r="G52" s="9"/>
+      <c r="H52" s="11"/>
+      <c r="I52" s="12"/>
+      <c r="J52" s="12"/>
+    </row>
+    <row r="53" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D53" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="E53" s="35">
+        <v>2.356789</v>
+      </c>
+      <c r="F53" s="35"/>
+      <c r="G53" s="22"/>
+      <c r="H53" s="17"/>
+      <c r="I53" s="3"/>
+    </row>
+    <row r="62" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C62" s="34"/>
+      <c r="D62" s="34"/>
+      <c r="F62" s="34"/>
+      <c r="G62" s="34"/>
+      <c r="H62" s="34"/>
+    </row>
+    <row r="63" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C63" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="D63" s="33"/>
+      <c r="F63" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="D56" s="44" t="s">
-        <v>18</v>
-      </c>
-      <c r="E56" s="44" t="s">
-        <v>19</v>
-      </c>
-      <c r="F56" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="G56" s="43" t="s">
-        <v>12</v>
-      </c>
-      <c r="H56" s="43" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="57" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B57" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="C57" s="16"/>
-      <c r="D57" s="6"/>
-      <c r="E57" s="6"/>
-      <c r="F57" s="23">
-        <v>2</v>
-      </c>
-      <c r="G57" s="23">
-        <v>2</v>
-      </c>
-      <c r="H57" s="24">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="58" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B58" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C58" s="16"/>
-      <c r="D58" s="6"/>
-      <c r="E58" s="6"/>
-      <c r="F58" s="23">
-        <v>2</v>
-      </c>
-      <c r="G58" s="23">
-        <v>2</v>
-      </c>
-      <c r="H58" s="24">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="59" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B59" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C59" s="16"/>
-      <c r="D59" s="7"/>
-      <c r="E59" s="7"/>
-      <c r="F59" s="25">
-        <v>3</v>
-      </c>
-      <c r="G59" s="25">
-        <v>3</v>
-      </c>
-      <c r="H59" s="26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B60" s="16"/>
-      <c r="C60" s="16"/>
-      <c r="D60" s="7"/>
-      <c r="E60" s="7"/>
-      <c r="F60" s="23"/>
-      <c r="G60" s="23">
-        <v>4</v>
-      </c>
-      <c r="H60" s="24">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="61" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B61" s="16"/>
-      <c r="C61" s="16"/>
-      <c r="D61" s="7"/>
-      <c r="E61" s="7"/>
-      <c r="F61" s="23"/>
-      <c r="G61" s="23">
-        <v>3</v>
-      </c>
-      <c r="H61" s="24">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="62" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B62" s="16"/>
-      <c r="C62" s="16"/>
-      <c r="D62" s="7"/>
-      <c r="E62" s="7"/>
-      <c r="F62" s="23"/>
-      <c r="G62" s="23">
-        <v>2</v>
-      </c>
-      <c r="H62" s="24">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="63" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B63" s="10"/>
-      <c r="C63" s="16"/>
-      <c r="D63" s="7"/>
-      <c r="E63" s="7"/>
-      <c r="F63" s="23"/>
-      <c r="G63" s="23">
-        <v>2</v>
-      </c>
-      <c r="H63" s="24">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="64" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B64" s="10"/>
-      <c r="C64" s="16"/>
-      <c r="D64" s="7"/>
-      <c r="E64" s="7"/>
-      <c r="F64" s="25"/>
-      <c r="G64" s="25">
-        <v>3</v>
-      </c>
-      <c r="H64" s="26">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="65" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B65" s="10"/>
-      <c r="C65" s="10"/>
-      <c r="D65" s="10"/>
-      <c r="E65" s="10"/>
-      <c r="F65" s="25"/>
-      <c r="G65" s="25"/>
-      <c r="H65" s="26"/>
-    </row>
-    <row r="66" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B66" s="9"/>
-      <c r="C66" s="20"/>
-      <c r="D66" s="9"/>
-      <c r="E66" s="9"/>
-      <c r="F66" s="14"/>
-      <c r="G66" s="14"/>
-      <c r="H66" s="14"/>
-    </row>
-    <row r="67" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B67" s="9"/>
-      <c r="C67" s="20"/>
-      <c r="D67" s="9"/>
-      <c r="E67" s="9"/>
-      <c r="F67" s="14"/>
-      <c r="G67" s="14"/>
-      <c r="H67" s="14"/>
-    </row>
-    <row r="68" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B68" s="9"/>
-      <c r="C68" s="20"/>
-      <c r="D68" s="9"/>
-      <c r="E68" s="9"/>
-      <c r="F68" s="14"/>
-      <c r="G68" s="14"/>
-      <c r="H68" s="14"/>
-    </row>
-    <row r="69" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D69" s="2"/>
-      <c r="E69" s="2"/>
-      <c r="F69" s="8"/>
-      <c r="G69" s="9"/>
-      <c r="H69" s="14"/>
-      <c r="I69" s="14"/>
-      <c r="J69" s="14"/>
-    </row>
-    <row r="70" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D70" s="8"/>
-      <c r="E70" s="8"/>
-      <c r="F70" s="8"/>
-      <c r="G70" s="9"/>
-      <c r="H70" s="11"/>
-      <c r="I70" s="12"/>
-      <c r="J70" s="12"/>
-    </row>
-    <row r="71" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D71" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="E71" s="40">
-        <v>2.356789</v>
-      </c>
-      <c r="F71" s="40"/>
-      <c r="G71" s="22"/>
-      <c r="H71" s="17"/>
-      <c r="I71" s="3"/>
-    </row>
-    <row r="80" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C80" s="39"/>
-      <c r="D80" s="39"/>
-      <c r="F80" s="39"/>
-      <c r="G80" s="39"/>
-      <c r="H80" s="39"/>
-    </row>
-    <row r="81" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C81" s="38" t="s">
-        <v>21</v>
-      </c>
-      <c r="D81" s="38"/>
-      <c r="F81" s="38" t="s">
-        <v>22</v>
-      </c>
-      <c r="G81" s="38"/>
-      <c r="H81" s="38"/>
+      <c r="G63" s="33"/>
+      <c r="H63" s="33"/>
     </row>
   </sheetData>
-  <mergeCells count="22">
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="C81:D81"/>
-    <mergeCell ref="F80:H80"/>
-    <mergeCell ref="F81:H81"/>
-    <mergeCell ref="C80:D80"/>
-    <mergeCell ref="E71:F71"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="D53:G54"/>
+  <mergeCells count="23">
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="A2:I2"/>
     <mergeCell ref="E4:F4"/>
@@ -3762,12 +2894,21 @@
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="G5:H5"/>
     <mergeCell ref="G6:H6"/>
-    <mergeCell ref="B36:B39"/>
-    <mergeCell ref="A8:I8"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C5:D5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="C63:D63"/>
+    <mergeCell ref="F62:H62"/>
+    <mergeCell ref="F63:H63"/>
+    <mergeCell ref="C62:D62"/>
+    <mergeCell ref="E53:F53"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="D35:G36"/>
+    <mergeCell ref="A10:I10"/>
+    <mergeCell ref="D34:G34"/>
+    <mergeCell ref="B8:H8"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="55" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>

</xml_diff>